<commit_message>
updated temoatools code to include discount rates
</commit_message>
<xml_diff>
--- a/virginia/data/data_virginia.xlsx
+++ b/virginia/data/data_virginia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077628C3-25EA-8645-A488-794B264BC5FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CDF7AF-A127-4C44-83E0-EA06614D577F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8960" yWindow="-21140" windowWidth="51200" windowHeight="21140" tabRatio="941" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="941" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -14,16 +14,17 @@
     <sheet name="Connections" sheetId="1" r:id="rId4"/>
     <sheet name="Demand" sheetId="3" r:id="rId5"/>
     <sheet name="ConnectionsExisting" sheetId="2" r:id="rId6"/>
-    <sheet name="DiscountRate" sheetId="5" r:id="rId7"/>
-    <sheet name="Fuels" sheetId="6" r:id="rId8"/>
-    <sheet name="FuelsExisting" sheetId="7" r:id="rId9"/>
-    <sheet name="PowerPlants" sheetId="8" r:id="rId10"/>
-    <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId11"/>
-    <sheet name="PowerPlantsCosts" sheetId="10" r:id="rId12"/>
-    <sheet name="PowerPlantsConstraints" sheetId="9" r:id="rId13"/>
-    <sheet name="PowerPlantsExisting" sheetId="11" r:id="rId14"/>
-    <sheet name="ReserveMargin" sheetId="13" r:id="rId15"/>
-    <sheet name="capacityFactorTOD" sheetId="14" r:id="rId16"/>
+    <sheet name="DiscountRateGlobal" sheetId="5" r:id="rId7"/>
+    <sheet name="DiscountRateTech" sheetId="19" r:id="rId8"/>
+    <sheet name="Fuels" sheetId="6" r:id="rId9"/>
+    <sheet name="FuelsExisting" sheetId="7" r:id="rId10"/>
+    <sheet name="PowerPlants" sheetId="8" r:id="rId11"/>
+    <sheet name="PowerPlantsPerformance" sheetId="12" r:id="rId12"/>
+    <sheet name="PowerPlantsCosts" sheetId="10" r:id="rId13"/>
+    <sheet name="PowerPlantsConstraints" sheetId="9" r:id="rId14"/>
+    <sheet name="PowerPlantsExisting" sheetId="11" r:id="rId15"/>
+    <sheet name="ReserveMargin" sheetId="13" r:id="rId16"/>
+    <sheet name="capacityFactorTOD" sheetId="14" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="237">
   <si>
     <t>connection</t>
   </si>
@@ -658,9 +659,6 @@
     <t>[fr]</t>
   </si>
   <si>
-    <t>10% discount rate Virginia</t>
-  </si>
-  <si>
     <t>https://www.eia.gov/state/?sid=VA#tabs-2 https://github.com/coopercenter/EO43/</t>
   </si>
   <si>
@@ -728,6 +726,27 @@
   </si>
   <si>
     <t>EIA</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>vintage</t>
+  </si>
+  <si>
+    <t>tech_rate</t>
+  </si>
+  <si>
+    <t>tech_rate_notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EC_WIND    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED_SOLPV   </t>
+  </si>
+  <si>
+    <t>8% discount rate Virginia</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1151,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1185,7 +1204,7 @@
         <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1193,7 +1212,7 @@
         <v>85</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G4" s="12"/>
     </row>
@@ -1213,10 +1232,10 @@
         <v>87</v>
       </c>
       <c r="C6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1224,10 +1243,10 @@
         <v>88</v>
       </c>
       <c r="C7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1235,10 +1254,10 @@
         <v>89</v>
       </c>
       <c r="C8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1246,10 +1265,10 @@
         <v>90</v>
       </c>
       <c r="C9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1362,7 +1381,7 @@
         <v>147</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1393,6 +1412,63 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3">
+        <v>3729</v>
+      </c>
+      <c r="C3">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -1727,10 +1803,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>103</v>
@@ -1779,7 +1855,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>103</v>
@@ -1805,7 +1881,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>121</v>
@@ -1831,7 +1907,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>103</v>
@@ -2271,7 +2347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -2590,7 +2666,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="5">
         <v>95</v>
@@ -2609,7 +2685,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" s="5">
         <v>56</v>
@@ -2634,7 +2710,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B15" s="5">
         <v>20</v>
@@ -2650,7 +2726,7 @@
         <v>100</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2703,7 +2779,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B18" s="16">
         <v>20</v>
@@ -2719,7 +2795,7 @@
         <v>100</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -3076,7 +3152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
@@ -3337,7 +3413,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3352,7 +3428,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="8"/>
@@ -3371,7 +3447,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="8"/>
@@ -3428,7 +3504,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B18" s="17">
         <v>3935</v>
@@ -3773,7 +3849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -3940,7 +4016,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13" s="5">
         <v>0.01</v>
@@ -3954,7 +4030,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3981,7 +4057,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -4159,11 +4235,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="M26" sqref="M26:M27"/>
     </sheetView>
   </sheetViews>
@@ -4213,7 +4289,7 @@
         <v>1985</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4249,7 +4325,7 @@
         <v>1980</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4291,7 +4367,7 @@
         <v>2010</v>
       </c>
       <c r="D9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4316,7 +4392,7 @@
         <v>1995</v>
       </c>
       <c r="D11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4330,7 +4406,7 @@
         <v>2016</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4344,7 +4420,7 @@
         <v>2015</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4358,12 +4434,12 @@
         <v>2015</v>
       </c>
       <c r="D14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B15">
         <v>3568</v>
@@ -4372,12 +4448,12 @@
         <v>2015</v>
       </c>
       <c r="D15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B16">
         <v>153</v>
@@ -4386,12 +4462,12 @@
         <v>2013</v>
       </c>
       <c r="D16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B17">
         <v>3200</v>
@@ -4400,7 +4476,7 @@
         <v>1970</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -4409,7 +4485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4450,7 +4526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E242"/>
   <sheetViews>
@@ -4505,7 +4581,7 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>170</v>
@@ -4522,7 +4598,7 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>171</v>
@@ -4539,7 +4615,7 @@
         <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>172</v>
@@ -4556,7 +4632,7 @@
         <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>173</v>
@@ -4573,7 +4649,7 @@
         <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>174</v>
@@ -4590,7 +4666,7 @@
         <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>175</v>
@@ -4607,7 +4683,7 @@
         <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>176</v>
@@ -4624,7 +4700,7 @@
         <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>177</v>
@@ -4641,7 +4717,7 @@
         <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>178</v>
@@ -4658,7 +4734,7 @@
         <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>49</v>
@@ -4675,7 +4751,7 @@
         <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>50</v>
@@ -4692,7 +4768,7 @@
         <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>51</v>
@@ -4709,7 +4785,7 @@
         <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>52</v>
@@ -4726,7 +4802,7 @@
         <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>53</v>
@@ -4743,7 +4819,7 @@
         <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>54</v>
@@ -4760,7 +4836,7 @@
         <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>55</v>
@@ -4777,7 +4853,7 @@
         <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>56</v>
@@ -4794,7 +4870,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>57</v>
@@ -4811,7 +4887,7 @@
         <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>58</v>
@@ -4828,7 +4904,7 @@
         <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>59</v>
@@ -4845,7 +4921,7 @@
         <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>60</v>
@@ -4862,7 +4938,7 @@
         <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>61</v>
@@ -4879,7 +4955,7 @@
         <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>62</v>
@@ -4896,7 +4972,7 @@
         <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>83</v>
@@ -4913,7 +4989,7 @@
         <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>170</v>
@@ -4930,7 +5006,7 @@
         <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>171</v>
@@ -4947,7 +5023,7 @@
         <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>172</v>
@@ -4964,7 +5040,7 @@
         <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>173</v>
@@ -4981,7 +5057,7 @@
         <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>174</v>
@@ -4998,7 +5074,7 @@
         <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>175</v>
@@ -5015,7 +5091,7 @@
         <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>176</v>
@@ -5032,7 +5108,7 @@
         <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>177</v>
@@ -5049,7 +5125,7 @@
         <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>178</v>
@@ -5066,7 +5142,7 @@
         <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>49</v>
@@ -5083,7 +5159,7 @@
         <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>50</v>
@@ -5100,7 +5176,7 @@
         <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>51</v>
@@ -5117,7 +5193,7 @@
         <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>52</v>
@@ -5134,7 +5210,7 @@
         <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>53</v>
@@ -5151,7 +5227,7 @@
         <v>93</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>54</v>
@@ -5168,7 +5244,7 @@
         <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>55</v>
@@ -5185,7 +5261,7 @@
         <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>56</v>
@@ -5202,7 +5278,7 @@
         <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>57</v>
@@ -5219,7 +5295,7 @@
         <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>58</v>
@@ -5236,7 +5312,7 @@
         <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>59</v>
@@ -5253,7 +5329,7 @@
         <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>60</v>
@@ -5270,7 +5346,7 @@
         <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>61</v>
@@ -5287,7 +5363,7 @@
         <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>62</v>
@@ -5304,7 +5380,7 @@
         <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>83</v>
@@ -5321,7 +5397,7 @@
         <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>170</v>
@@ -5338,7 +5414,7 @@
         <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>171</v>
@@ -5355,7 +5431,7 @@
         <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>172</v>
@@ -5372,7 +5448,7 @@
         <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>173</v>
@@ -5389,7 +5465,7 @@
         <v>93</v>
       </c>
       <c r="B55" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>174</v>
@@ -5406,7 +5482,7 @@
         <v>93</v>
       </c>
       <c r="B56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>175</v>
@@ -5423,7 +5499,7 @@
         <v>93</v>
       </c>
       <c r="B57" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>176</v>
@@ -5440,7 +5516,7 @@
         <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>177</v>
@@ -5457,7 +5533,7 @@
         <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>178</v>
@@ -5474,7 +5550,7 @@
         <v>93</v>
       </c>
       <c r="B60" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>49</v>
@@ -5491,7 +5567,7 @@
         <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>50</v>
@@ -5508,7 +5584,7 @@
         <v>93</v>
       </c>
       <c r="B62" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>51</v>
@@ -5525,7 +5601,7 @@
         <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>52</v>
@@ -5542,7 +5618,7 @@
         <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>53</v>
@@ -5559,7 +5635,7 @@
         <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>54</v>
@@ -5576,7 +5652,7 @@
         <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>55</v>
@@ -5593,7 +5669,7 @@
         <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>56</v>
@@ -5610,7 +5686,7 @@
         <v>93</v>
       </c>
       <c r="B68" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>57</v>
@@ -5627,7 +5703,7 @@
         <v>93</v>
       </c>
       <c r="B69" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>58</v>
@@ -5644,7 +5720,7 @@
         <v>93</v>
       </c>
       <c r="B70" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>59</v>
@@ -5661,7 +5737,7 @@
         <v>93</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>60</v>
@@ -5678,7 +5754,7 @@
         <v>93</v>
       </c>
       <c r="B72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>61</v>
@@ -5695,7 +5771,7 @@
         <v>93</v>
       </c>
       <c r="B73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>62</v>
@@ -5712,7 +5788,7 @@
         <v>93</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>83</v>
@@ -5729,7 +5805,7 @@
         <v>93</v>
       </c>
       <c r="B75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>170</v>
@@ -5746,7 +5822,7 @@
         <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>171</v>
@@ -5763,7 +5839,7 @@
         <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>172</v>
@@ -5780,7 +5856,7 @@
         <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>173</v>
@@ -5797,7 +5873,7 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C79" s="15" t="s">
         <v>174</v>
@@ -5814,7 +5890,7 @@
         <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>175</v>
@@ -5831,7 +5907,7 @@
         <v>93</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>176</v>
@@ -5848,7 +5924,7 @@
         <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>177</v>
@@ -5865,7 +5941,7 @@
         <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>178</v>
@@ -5882,7 +5958,7 @@
         <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>49</v>
@@ -5899,7 +5975,7 @@
         <v>93</v>
       </c>
       <c r="B85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>50</v>
@@ -5916,7 +5992,7 @@
         <v>93</v>
       </c>
       <c r="B86" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>51</v>
@@ -5933,7 +6009,7 @@
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>52</v>
@@ -5950,7 +6026,7 @@
         <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>53</v>
@@ -5967,7 +6043,7 @@
         <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>54</v>
@@ -5984,7 +6060,7 @@
         <v>93</v>
       </c>
       <c r="B90" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C90" s="15" t="s">
         <v>55</v>
@@ -6001,7 +6077,7 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>56</v>
@@ -6018,7 +6094,7 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C92" s="15" t="s">
         <v>57</v>
@@ -6035,7 +6111,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>58</v>
@@ -6052,7 +6128,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>59</v>
@@ -6069,7 +6145,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>60</v>
@@ -6086,7 +6162,7 @@
         <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>61</v>
@@ -6103,7 +6179,7 @@
         <v>93</v>
       </c>
       <c r="B97" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C97" s="15" t="s">
         <v>62</v>
@@ -6120,7 +6196,7 @@
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>83</v>
@@ -6137,7 +6213,7 @@
         <v>93</v>
       </c>
       <c r="B99" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C99" s="15" t="s">
         <v>170</v>
@@ -6154,7 +6230,7 @@
         <v>93</v>
       </c>
       <c r="B100" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C100" s="15" t="s">
         <v>171</v>
@@ -6171,7 +6247,7 @@
         <v>93</v>
       </c>
       <c r="B101" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C101" s="15" t="s">
         <v>172</v>
@@ -6188,7 +6264,7 @@
         <v>93</v>
       </c>
       <c r="B102" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C102" s="15" t="s">
         <v>173</v>
@@ -6205,7 +6281,7 @@
         <v>93</v>
       </c>
       <c r="B103" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C103" s="15" t="s">
         <v>174</v>
@@ -6222,7 +6298,7 @@
         <v>93</v>
       </c>
       <c r="B104" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C104" s="15" t="s">
         <v>175</v>
@@ -6239,7 +6315,7 @@
         <v>93</v>
       </c>
       <c r="B105" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>176</v>
@@ -6256,7 +6332,7 @@
         <v>93</v>
       </c>
       <c r="B106" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C106" s="15" t="s">
         <v>177</v>
@@ -6273,7 +6349,7 @@
         <v>93</v>
       </c>
       <c r="B107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C107" s="15" t="s">
         <v>178</v>
@@ -6290,7 +6366,7 @@
         <v>93</v>
       </c>
       <c r="B108" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C108" s="15" t="s">
         <v>49</v>
@@ -6307,7 +6383,7 @@
         <v>93</v>
       </c>
       <c r="B109" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C109" s="15" t="s">
         <v>50</v>
@@ -6324,7 +6400,7 @@
         <v>93</v>
       </c>
       <c r="B110" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>51</v>
@@ -6341,7 +6417,7 @@
         <v>93</v>
       </c>
       <c r="B111" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C111" s="15" t="s">
         <v>52</v>
@@ -6358,7 +6434,7 @@
         <v>93</v>
       </c>
       <c r="B112" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C112" s="15" t="s">
         <v>53</v>
@@ -6375,7 +6451,7 @@
         <v>93</v>
       </c>
       <c r="B113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C113" s="15" t="s">
         <v>54</v>
@@ -6392,7 +6468,7 @@
         <v>93</v>
       </c>
       <c r="B114" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C114" s="15" t="s">
         <v>55</v>
@@ -6409,7 +6485,7 @@
         <v>93</v>
       </c>
       <c r="B115" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C115" s="15" t="s">
         <v>56</v>
@@ -6426,7 +6502,7 @@
         <v>93</v>
       </c>
       <c r="B116" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C116" s="15" t="s">
         <v>57</v>
@@ -6443,7 +6519,7 @@
         <v>93</v>
       </c>
       <c r="B117" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C117" s="15" t="s">
         <v>58</v>
@@ -6460,7 +6536,7 @@
         <v>93</v>
       </c>
       <c r="B118" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C118" s="15" t="s">
         <v>59</v>
@@ -6477,7 +6553,7 @@
         <v>93</v>
       </c>
       <c r="B119" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C119" s="15" t="s">
         <v>60</v>
@@ -6494,7 +6570,7 @@
         <v>93</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C120" s="15" t="s">
         <v>61</v>
@@ -6511,7 +6587,7 @@
         <v>93</v>
       </c>
       <c r="B121" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C121" s="15" t="s">
         <v>62</v>
@@ -6528,7 +6604,7 @@
         <v>93</v>
       </c>
       <c r="B122" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C122" s="15" t="s">
         <v>83</v>
@@ -6545,7 +6621,7 @@
         <v>94</v>
       </c>
       <c r="B123" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C123" s="15" t="s">
         <v>170</v>
@@ -6562,7 +6638,7 @@
         <v>94</v>
       </c>
       <c r="B124" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C124" s="15" t="s">
         <v>171</v>
@@ -6579,7 +6655,7 @@
         <v>94</v>
       </c>
       <c r="B125" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C125" s="15" t="s">
         <v>172</v>
@@ -6596,7 +6672,7 @@
         <v>94</v>
       </c>
       <c r="B126" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C126" s="15" t="s">
         <v>173</v>
@@ -6613,7 +6689,7 @@
         <v>94</v>
       </c>
       <c r="B127" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C127" s="15" t="s">
         <v>174</v>
@@ -6630,7 +6706,7 @@
         <v>94</v>
       </c>
       <c r="B128" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C128" s="15" t="s">
         <v>175</v>
@@ -6647,7 +6723,7 @@
         <v>94</v>
       </c>
       <c r="B129" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C129" s="15" t="s">
         <v>176</v>
@@ -6664,7 +6740,7 @@
         <v>94</v>
       </c>
       <c r="B130" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C130" s="15" t="s">
         <v>177</v>
@@ -6681,7 +6757,7 @@
         <v>94</v>
       </c>
       <c r="B131" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C131" s="15" t="s">
         <v>178</v>
@@ -6698,7 +6774,7 @@
         <v>94</v>
       </c>
       <c r="B132" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C132" s="15" t="s">
         <v>49</v>
@@ -6715,7 +6791,7 @@
         <v>94</v>
       </c>
       <c r="B133" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C133" s="15" t="s">
         <v>50</v>
@@ -6732,7 +6808,7 @@
         <v>94</v>
       </c>
       <c r="B134" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C134" s="15" t="s">
         <v>51</v>
@@ -6749,7 +6825,7 @@
         <v>94</v>
       </c>
       <c r="B135" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C135" s="15" t="s">
         <v>52</v>
@@ -6766,7 +6842,7 @@
         <v>94</v>
       </c>
       <c r="B136" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C136" s="15" t="s">
         <v>53</v>
@@ -6783,7 +6859,7 @@
         <v>94</v>
       </c>
       <c r="B137" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C137" s="15" t="s">
         <v>54</v>
@@ -6800,7 +6876,7 @@
         <v>94</v>
       </c>
       <c r="B138" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C138" s="15" t="s">
         <v>55</v>
@@ -6817,7 +6893,7 @@
         <v>94</v>
       </c>
       <c r="B139" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C139" s="15" t="s">
         <v>56</v>
@@ -6834,7 +6910,7 @@
         <v>94</v>
       </c>
       <c r="B140" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C140" s="15" t="s">
         <v>57</v>
@@ -6851,7 +6927,7 @@
         <v>94</v>
       </c>
       <c r="B141" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C141" s="15" t="s">
         <v>58</v>
@@ -6868,7 +6944,7 @@
         <v>94</v>
       </c>
       <c r="B142" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C142" s="15" t="s">
         <v>59</v>
@@ -6885,7 +6961,7 @@
         <v>94</v>
       </c>
       <c r="B143" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C143" s="15" t="s">
         <v>60</v>
@@ -6902,7 +6978,7 @@
         <v>94</v>
       </c>
       <c r="B144" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C144" s="15" t="s">
         <v>61</v>
@@ -6919,7 +6995,7 @@
         <v>94</v>
       </c>
       <c r="B145" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C145" s="15" t="s">
         <v>62</v>
@@ -6936,7 +7012,7 @@
         <v>94</v>
       </c>
       <c r="B146" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C146" s="15" t="s">
         <v>83</v>
@@ -6953,7 +7029,7 @@
         <v>94</v>
       </c>
       <c r="B147" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C147" s="15" t="s">
         <v>170</v>
@@ -6970,7 +7046,7 @@
         <v>94</v>
       </c>
       <c r="B148" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C148" s="15" t="s">
         <v>171</v>
@@ -6987,7 +7063,7 @@
         <v>94</v>
       </c>
       <c r="B149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C149" s="15" t="s">
         <v>172</v>
@@ -7004,7 +7080,7 @@
         <v>94</v>
       </c>
       <c r="B150" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C150" s="15" t="s">
         <v>173</v>
@@ -7021,7 +7097,7 @@
         <v>94</v>
       </c>
       <c r="B151" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C151" s="15" t="s">
         <v>174</v>
@@ -7038,7 +7114,7 @@
         <v>94</v>
       </c>
       <c r="B152" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C152" s="15" t="s">
         <v>175</v>
@@ -7055,7 +7131,7 @@
         <v>94</v>
       </c>
       <c r="B153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C153" s="15" t="s">
         <v>176</v>
@@ -7072,7 +7148,7 @@
         <v>94</v>
       </c>
       <c r="B154" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C154" s="15" t="s">
         <v>177</v>
@@ -7089,7 +7165,7 @@
         <v>94</v>
       </c>
       <c r="B155" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C155" s="15" t="s">
         <v>178</v>
@@ -7106,7 +7182,7 @@
         <v>94</v>
       </c>
       <c r="B156" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C156" s="15" t="s">
         <v>49</v>
@@ -7123,7 +7199,7 @@
         <v>94</v>
       </c>
       <c r="B157" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C157" s="15" t="s">
         <v>50</v>
@@ -7140,7 +7216,7 @@
         <v>94</v>
       </c>
       <c r="B158" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C158" s="15" t="s">
         <v>51</v>
@@ -7157,7 +7233,7 @@
         <v>94</v>
       </c>
       <c r="B159" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C159" s="15" t="s">
         <v>52</v>
@@ -7174,7 +7250,7 @@
         <v>94</v>
       </c>
       <c r="B160" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C160" s="15" t="s">
         <v>53</v>
@@ -7191,7 +7267,7 @@
         <v>94</v>
       </c>
       <c r="B161" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C161" s="15" t="s">
         <v>54</v>
@@ -7208,7 +7284,7 @@
         <v>94</v>
       </c>
       <c r="B162" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C162" s="15" t="s">
         <v>55</v>
@@ -7225,7 +7301,7 @@
         <v>94</v>
       </c>
       <c r="B163" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C163" s="15" t="s">
         <v>56</v>
@@ -7242,7 +7318,7 @@
         <v>94</v>
       </c>
       <c r="B164" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C164" s="15" t="s">
         <v>57</v>
@@ -7259,7 +7335,7 @@
         <v>94</v>
       </c>
       <c r="B165" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C165" s="15" t="s">
         <v>58</v>
@@ -7276,7 +7352,7 @@
         <v>94</v>
       </c>
       <c r="B166" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C166" s="15" t="s">
         <v>59</v>
@@ -7293,7 +7369,7 @@
         <v>94</v>
       </c>
       <c r="B167" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C167" s="15" t="s">
         <v>60</v>
@@ -7310,7 +7386,7 @@
         <v>94</v>
       </c>
       <c r="B168" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C168" s="15" t="s">
         <v>61</v>
@@ -7327,7 +7403,7 @@
         <v>94</v>
       </c>
       <c r="B169" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C169" s="15" t="s">
         <v>62</v>
@@ -7344,7 +7420,7 @@
         <v>94</v>
       </c>
       <c r="B170" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C170" s="15" t="s">
         <v>83</v>
@@ -7361,7 +7437,7 @@
         <v>94</v>
       </c>
       <c r="B171" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C171" s="15" t="s">
         <v>170</v>
@@ -7378,7 +7454,7 @@
         <v>94</v>
       </c>
       <c r="B172" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C172" s="15" t="s">
         <v>171</v>
@@ -7395,7 +7471,7 @@
         <v>94</v>
       </c>
       <c r="B173" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C173" s="15" t="s">
         <v>172</v>
@@ -7412,7 +7488,7 @@
         <v>94</v>
       </c>
       <c r="B174" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C174" s="15" t="s">
         <v>173</v>
@@ -7429,7 +7505,7 @@
         <v>94</v>
       </c>
       <c r="B175" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C175" s="15" t="s">
         <v>174</v>
@@ -7446,7 +7522,7 @@
         <v>94</v>
       </c>
       <c r="B176" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C176" s="15" t="s">
         <v>175</v>
@@ -7463,7 +7539,7 @@
         <v>94</v>
       </c>
       <c r="B177" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C177" s="15" t="s">
         <v>176</v>
@@ -7480,7 +7556,7 @@
         <v>94</v>
       </c>
       <c r="B178" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C178" s="15" t="s">
         <v>177</v>
@@ -7497,7 +7573,7 @@
         <v>94</v>
       </c>
       <c r="B179" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C179" s="15" t="s">
         <v>178</v>
@@ -7514,7 +7590,7 @@
         <v>94</v>
       </c>
       <c r="B180" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C180" s="15" t="s">
         <v>49</v>
@@ -7531,7 +7607,7 @@
         <v>94</v>
       </c>
       <c r="B181" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C181" s="15" t="s">
         <v>50</v>
@@ -7548,7 +7624,7 @@
         <v>94</v>
       </c>
       <c r="B182" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C182" s="15" t="s">
         <v>51</v>
@@ -7565,7 +7641,7 @@
         <v>94</v>
       </c>
       <c r="B183" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C183" s="15" t="s">
         <v>52</v>
@@ -7582,7 +7658,7 @@
         <v>94</v>
       </c>
       <c r="B184" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C184" s="15" t="s">
         <v>53</v>
@@ -7599,7 +7675,7 @@
         <v>94</v>
       </c>
       <c r="B185" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C185" s="15" t="s">
         <v>54</v>
@@ -7616,7 +7692,7 @@
         <v>94</v>
       </c>
       <c r="B186" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C186" s="15" t="s">
         <v>55</v>
@@ -7633,7 +7709,7 @@
         <v>94</v>
       </c>
       <c r="B187" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C187" s="15" t="s">
         <v>56</v>
@@ -7650,7 +7726,7 @@
         <v>94</v>
       </c>
       <c r="B188" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C188" s="15" t="s">
         <v>57</v>
@@ -7667,7 +7743,7 @@
         <v>94</v>
       </c>
       <c r="B189" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C189" s="15" t="s">
         <v>58</v>
@@ -7684,7 +7760,7 @@
         <v>94</v>
       </c>
       <c r="B190" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C190" s="15" t="s">
         <v>59</v>
@@ -7701,7 +7777,7 @@
         <v>94</v>
       </c>
       <c r="B191" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C191" s="15" t="s">
         <v>60</v>
@@ -7718,7 +7794,7 @@
         <v>94</v>
       </c>
       <c r="B192" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C192" s="15" t="s">
         <v>61</v>
@@ -7735,7 +7811,7 @@
         <v>94</v>
       </c>
       <c r="B193" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C193" s="15" t="s">
         <v>62</v>
@@ -7752,7 +7828,7 @@
         <v>94</v>
       </c>
       <c r="B194" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C194" s="15" t="s">
         <v>83</v>
@@ -7769,7 +7845,7 @@
         <v>94</v>
       </c>
       <c r="B195" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C195" s="15" t="s">
         <v>170</v>
@@ -7786,7 +7862,7 @@
         <v>94</v>
       </c>
       <c r="B196" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C196" s="15" t="s">
         <v>171</v>
@@ -7803,7 +7879,7 @@
         <v>94</v>
       </c>
       <c r="B197" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C197" s="15" t="s">
         <v>172</v>
@@ -7820,7 +7896,7 @@
         <v>94</v>
       </c>
       <c r="B198" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C198" s="15" t="s">
         <v>173</v>
@@ -7837,7 +7913,7 @@
         <v>94</v>
       </c>
       <c r="B199" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C199" s="15" t="s">
         <v>174</v>
@@ -7854,7 +7930,7 @@
         <v>94</v>
       </c>
       <c r="B200" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C200" s="15" t="s">
         <v>175</v>
@@ -7871,7 +7947,7 @@
         <v>94</v>
       </c>
       <c r="B201" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C201" s="15" t="s">
         <v>176</v>
@@ -7888,7 +7964,7 @@
         <v>94</v>
       </c>
       <c r="B202" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C202" s="15" t="s">
         <v>177</v>
@@ -7905,7 +7981,7 @@
         <v>94</v>
       </c>
       <c r="B203" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C203" s="15" t="s">
         <v>178</v>
@@ -7922,7 +7998,7 @@
         <v>94</v>
       </c>
       <c r="B204" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C204" s="15" t="s">
         <v>49</v>
@@ -7939,7 +8015,7 @@
         <v>94</v>
       </c>
       <c r="B205" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C205" s="15" t="s">
         <v>50</v>
@@ -7956,7 +8032,7 @@
         <v>94</v>
       </c>
       <c r="B206" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C206" s="15" t="s">
         <v>51</v>
@@ -7973,7 +8049,7 @@
         <v>94</v>
       </c>
       <c r="B207" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C207" s="15" t="s">
         <v>52</v>
@@ -7990,7 +8066,7 @@
         <v>94</v>
       </c>
       <c r="B208" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C208" s="15" t="s">
         <v>53</v>
@@ -8007,7 +8083,7 @@
         <v>94</v>
       </c>
       <c r="B209" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C209" s="15" t="s">
         <v>54</v>
@@ -8024,7 +8100,7 @@
         <v>94</v>
       </c>
       <c r="B210" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C210" s="15" t="s">
         <v>55</v>
@@ -8041,7 +8117,7 @@
         <v>94</v>
       </c>
       <c r="B211" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C211" s="15" t="s">
         <v>56</v>
@@ -8058,7 +8134,7 @@
         <v>94</v>
       </c>
       <c r="B212" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C212" s="15" t="s">
         <v>57</v>
@@ -8075,7 +8151,7 @@
         <v>94</v>
       </c>
       <c r="B213" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C213" s="15" t="s">
         <v>58</v>
@@ -8092,7 +8168,7 @@
         <v>94</v>
       </c>
       <c r="B214" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C214" s="15" t="s">
         <v>59</v>
@@ -8109,7 +8185,7 @@
         <v>94</v>
       </c>
       <c r="B215" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C215" s="15" t="s">
         <v>60</v>
@@ -8126,7 +8202,7 @@
         <v>94</v>
       </c>
       <c r="B216" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C216" s="15" t="s">
         <v>61</v>
@@ -8143,7 +8219,7 @@
         <v>94</v>
       </c>
       <c r="B217" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C217" s="15" t="s">
         <v>62</v>
@@ -8160,7 +8236,7 @@
         <v>94</v>
       </c>
       <c r="B218" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C218" s="15" t="s">
         <v>83</v>
@@ -8177,7 +8253,7 @@
         <v>94</v>
       </c>
       <c r="B219" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C219" s="15" t="s">
         <v>170</v>
@@ -8194,7 +8270,7 @@
         <v>94</v>
       </c>
       <c r="B220" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C220" s="15" t="s">
         <v>171</v>
@@ -8211,7 +8287,7 @@
         <v>94</v>
       </c>
       <c r="B221" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C221" s="15" t="s">
         <v>172</v>
@@ -8228,7 +8304,7 @@
         <v>94</v>
       </c>
       <c r="B222" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C222" s="15" t="s">
         <v>173</v>
@@ -8245,7 +8321,7 @@
         <v>94</v>
       </c>
       <c r="B223" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C223" s="15" t="s">
         <v>174</v>
@@ -8262,7 +8338,7 @@
         <v>94</v>
       </c>
       <c r="B224" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C224" s="15" t="s">
         <v>175</v>
@@ -8279,7 +8355,7 @@
         <v>94</v>
       </c>
       <c r="B225" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C225" s="15" t="s">
         <v>176</v>
@@ -8296,7 +8372,7 @@
         <v>94</v>
       </c>
       <c r="B226" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C226" s="15" t="s">
         <v>177</v>
@@ -8313,7 +8389,7 @@
         <v>94</v>
       </c>
       <c r="B227" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C227" s="15" t="s">
         <v>178</v>
@@ -8330,7 +8406,7 @@
         <v>94</v>
       </c>
       <c r="B228" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C228" s="15" t="s">
         <v>49</v>
@@ -8347,7 +8423,7 @@
         <v>94</v>
       </c>
       <c r="B229" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C229" s="15" t="s">
         <v>50</v>
@@ -8364,7 +8440,7 @@
         <v>94</v>
       </c>
       <c r="B230" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C230" s="15" t="s">
         <v>51</v>
@@ -8381,7 +8457,7 @@
         <v>94</v>
       </c>
       <c r="B231" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C231" s="15" t="s">
         <v>52</v>
@@ -8398,7 +8474,7 @@
         <v>94</v>
       </c>
       <c r="B232" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C232" s="15" t="s">
         <v>53</v>
@@ -8415,7 +8491,7 @@
         <v>94</v>
       </c>
       <c r="B233" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C233" s="15" t="s">
         <v>54</v>
@@ -8432,7 +8508,7 @@
         <v>94</v>
       </c>
       <c r="B234" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C234" s="15" t="s">
         <v>55</v>
@@ -8449,7 +8525,7 @@
         <v>94</v>
       </c>
       <c r="B235" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C235" s="15" t="s">
         <v>56</v>
@@ -8466,7 +8542,7 @@
         <v>94</v>
       </c>
       <c r="B236" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C236" s="15" t="s">
         <v>57</v>
@@ -8483,7 +8559,7 @@
         <v>94</v>
       </c>
       <c r="B237" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C237" s="15" t="s">
         <v>58</v>
@@ -8500,7 +8576,7 @@
         <v>94</v>
       </c>
       <c r="B238" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C238" s="15" t="s">
         <v>59</v>
@@ -8517,7 +8593,7 @@
         <v>94</v>
       </c>
       <c r="B239" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C239" s="15" t="s">
         <v>60</v>
@@ -8534,7 +8610,7 @@
         <v>94</v>
       </c>
       <c r="B240" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C240" s="15" t="s">
         <v>61</v>
@@ -8551,7 +8627,7 @@
         <v>94</v>
       </c>
       <c r="B241" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C241" s="15" t="s">
         <v>62</v>
@@ -8568,7 +8644,7 @@
         <v>94</v>
       </c>
       <c r="B242" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C242" s="15" t="s">
         <v>83</v>
@@ -8624,7 +8700,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -8635,7 +8711,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B4">
         <v>0.32</v>
@@ -8646,7 +8722,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5">
         <v>0.2</v>
@@ -8657,7 +8733,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B6">
         <v>0.224</v>
@@ -8668,7 +8744,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7">
         <v>5.6000000000000001E-2</v>
@@ -9708,7 +9784,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9747,6 +9823,349 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCEDF73-15BA-AB46-9BE9-827A810B084A}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:C51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="C3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4">
+        <v>2025</v>
+      </c>
+      <c r="C4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5">
+        <v>2030</v>
+      </c>
+      <c r="C5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6">
+        <v>2035</v>
+      </c>
+      <c r="C6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7">
+        <v>2040</v>
+      </c>
+      <c r="C7">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8">
+        <v>2045</v>
+      </c>
+      <c r="C8">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9">
+        <v>2050</v>
+      </c>
+      <c r="C9">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10">
+        <v>2020</v>
+      </c>
+      <c r="C10">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11">
+        <v>2025</v>
+      </c>
+      <c r="C11">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12">
+        <v>2030</v>
+      </c>
+      <c r="C12">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13">
+        <v>2035</v>
+      </c>
+      <c r="C13">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14">
+        <v>2040</v>
+      </c>
+      <c r="C14">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15">
+        <v>2045</v>
+      </c>
+      <c r="C15">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B16">
+        <v>2050</v>
+      </c>
+      <c r="C16">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17">
+        <v>2020</v>
+      </c>
+      <c r="C17">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18">
+        <v>2025</v>
+      </c>
+      <c r="C18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B19">
+        <v>2030</v>
+      </c>
+      <c r="C19">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20">
+        <v>2035</v>
+      </c>
+      <c r="C20">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>235</v>
+      </c>
+      <c r="B21">
+        <v>2040</v>
+      </c>
+      <c r="C21">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22">
+        <v>2045</v>
+      </c>
+      <c r="C22">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23">
+        <v>2050</v>
+      </c>
+      <c r="C23">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24">
+        <v>2020</v>
+      </c>
+      <c r="C24">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25">
+        <v>2025</v>
+      </c>
+      <c r="C25">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26">
+        <v>2030</v>
+      </c>
+      <c r="C26">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27">
+        <v>2035</v>
+      </c>
+      <c r="C27">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28">
+        <v>2040</v>
+      </c>
+      <c r="C28">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <v>2045</v>
+      </c>
+      <c r="C29">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30">
+        <v>2050</v>
+      </c>
+      <c r="C30">
+        <v>0.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -10054,7 +10473,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12">
         <v>1.94</v>
@@ -10067,61 +10486,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3">
-        <v>3729</v>
-      </c>
-      <c r="C3">
-        <v>2015</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
minor value update / reduced senario
</commit_message>
<xml_diff>
--- a/virginia/data/data_virginia.xlsx
+++ b/virginia/data/data_virginia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309D46DA-4409-F74B-B8E1-ADA7F991E460}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451EE38F-8154-5F45-8E71-9B67B37774B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="21100" tabRatio="941" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="500" windowWidth="25600" windowHeight="21100" tabRatio="844" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="260">
   <si>
     <t>connection</t>
   </si>
@@ -793,27 +793,15 @@
     <t>Luo [Mid Value]</t>
   </si>
   <si>
-    <t>Assuming similar to Bath County</t>
-  </si>
-  <si>
     <t>NREL ATB (NPD 4)</t>
   </si>
   <si>
-    <t>Vennemann 2010</t>
-  </si>
-  <si>
     <t>Immendoerfer 2017</t>
   </si>
   <si>
-    <t>Abdulgafar 2014</t>
-  </si>
-  <si>
     <t>Rehman 2015</t>
   </si>
   <si>
-    <t>https://www.eia.gov/state/seds/sep_fuel/html/pdf/fuel_pr_ww.pdf</t>
-  </si>
-  <si>
     <t>https://www.eia.gov/outlooks/aeo/data/browser/#/?id=15-AEO2020&amp;cases=ref2020&amp;sourcekey=0</t>
   </si>
   <si>
@@ -821,6 +809,15 @@
   </si>
   <si>
     <t>NREL ATB &amp; https://www.eia.gov/outlooks/aeo/data/browser/#/?id=12-AEO2020&amp;cases=ref2020&amp;sourcekey=0</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/state/seds/sep_fuel/html/pdf/fuel_pr_ww.pdf, NREL ATB</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/pv/assets/pdfs/champion-module-efficiencies.20200708.pdf</t>
+  </si>
+  <si>
+    <t>Beuse et al.</t>
   </si>
 </sst>
 </file>
@@ -829,9 +826,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -869,18 +866,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -900,8 +885,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -911,18 +929,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,6 +949,34 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -953,13 +987,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -975,33 +1011,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -1559,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1637,10 +1704,10 @@
       <c r="Q1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1696,10 +1763,10 @@
       <c r="Q2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="R2" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="S2" s="21" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1707,11 +1774,11 @@
       <c r="A3" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="35">
-        <v>2.86</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="B3" s="59">
+        <v>2.85</v>
+      </c>
+      <c r="C3" s="44">
+        <v>0</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>257</v>
@@ -1726,11 +1793,11 @@
       <c r="K3" t="s">
         <v>154</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="21">
         <f>14.35*2.99</f>
         <v>42.906500000000001</v>
       </c>
-      <c r="Q3" s="29" t="s">
+      <c r="Q3" s="21" t="s">
         <v>249</v>
       </c>
     </row>
@@ -1738,17 +1805,17 @@
       <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="35">
-        <v>1.95</v>
-      </c>
-      <c r="C4" s="35">
+      <c r="B4" s="23">
+        <v>2.75</v>
+      </c>
+      <c r="C4" s="25">
         <v>-0.1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H4">
-        <v>90.37</v>
+        <v>88.43</v>
       </c>
       <c r="I4" t="s">
         <v>87</v>
@@ -1764,9 +1831,10 @@
       <c r="A5" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
+      <c r="B5" s="24">
+        <v>0</v>
+      </c>
+      <c r="C5" s="24"/>
       <c r="J5">
         <v>50</v>
       </c>
@@ -1778,14 +1846,14 @@
       <c r="A6" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="35">
-        <v>14.6</v>
-      </c>
-      <c r="C6" s="35">
+      <c r="B6" s="23">
+        <v>11.29</v>
+      </c>
+      <c r="C6" s="25">
         <v>3.6</v>
       </c>
       <c r="D6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="H6">
         <v>67.58</v>
@@ -1804,14 +1872,14 @@
       <c r="A7" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="35">
-        <v>2.79</v>
-      </c>
-      <c r="C7" s="35">
+      <c r="B7" s="23">
+        <v>3.91</v>
+      </c>
+      <c r="C7" s="25">
         <v>1.1000000000000001</v>
       </c>
       <c r="D7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H7">
         <v>50.3</v>
@@ -1825,17 +1893,17 @@
       <c r="K7" t="s">
         <v>154</v>
       </c>
-      <c r="P7" s="29">
+      <c r="P7" s="21">
         <f>300.68*1.11</f>
         <v>333.75480000000005</v>
       </c>
-      <c r="Q7" s="29" t="s">
+      <c r="Q7" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="R7" s="29">
+      <c r="R7" s="21">
         <v>19890</v>
       </c>
-      <c r="S7" s="29" t="s">
+      <c r="S7" s="21" t="s">
         <v>247</v>
       </c>
     </row>
@@ -1843,9 +1911,10 @@
       <c r="A8" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
+      <c r="B8" s="24">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12"/>
       <c r="J8">
         <v>50</v>
       </c>
@@ -1857,9 +1926,10 @@
       <c r="A9" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
+      <c r="B9" s="24">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12"/>
       <c r="J9">
         <v>50</v>
       </c>
@@ -1871,13 +1941,13 @@
       <c r="A10" t="s">
         <v>185</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="35" t="s">
+      <c r="B10" s="58">
+        <v>0.63</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>183</v>
       </c>
       <c r="J10">
@@ -1886,6 +1956,10 @@
       <c r="K10" t="s">
         <v>154</v>
       </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1950,7 +2024,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2058,14 +2132,14 @@
       <c r="H3" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="13">
         <v>0.9</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="16">
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
         <v>237</v>
       </c>
@@ -2090,10 +2164,10 @@
       <c r="H4" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="60">
         <v>0.95</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2122,10 +2196,10 @@
       <c r="H5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="13">
         <v>0.95</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2154,14 +2228,14 @@
       <c r="H6" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="13">
         <v>0.95</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="16">
+      <c r="K6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="5" t="s">
         <v>238</v>
       </c>
@@ -2186,14 +2260,14 @@
       <c r="H7" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="60">
         <v>0.91</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="16">
+      <c r="K7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="5" t="s">
         <v>106</v>
       </c>
@@ -2218,11 +2292,11 @@
       <c r="H8" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="35">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="K8" s="35">
-        <v>0</v>
+      <c r="J8" s="61">
+        <v>0.37</v>
+      </c>
+      <c r="K8" s="61">
+        <v>-3.68</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2250,14 +2324,14 @@
       <c r="H9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="13">
         <v>0.98</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="16">
+      <c r="K9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
         <v>107</v>
       </c>
@@ -2282,14 +2356,14 @@
       <c r="H10" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J10" s="35">
-        <v>0.44</v>
-      </c>
-      <c r="K10" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="16">
+      <c r="J10" s="61">
+        <v>0.51</v>
+      </c>
+      <c r="K10" s="61">
+        <v>-2.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
         <v>202</v>
       </c>
@@ -2303,7 +2377,7 @@
         <v>119</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>118</v>
@@ -2317,10 +2391,10 @@
       <c r="I11">
         <v>12</v>
       </c>
-      <c r="J11" s="35">
+      <c r="J11" s="60">
         <v>0.95</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2349,14 +2423,14 @@
       <c r="H12" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="13">
         <v>0.95</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="16">
+      <c r="K12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="14" t="s">
         <v>203</v>
       </c>
@@ -2370,7 +2444,7 @@
         <v>119</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>119</v>
@@ -2384,10 +2458,10 @@
       <c r="I13">
         <v>12</v>
       </c>
-      <c r="J13" s="35">
+      <c r="J13" s="60">
         <v>0.95</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2405,7 +2479,7 @@
         <v>119</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>119</v>
@@ -2419,14 +2493,14 @@
       <c r="I14">
         <v>4</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="13">
         <v>0.75</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="16">
+      <c r="K14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="14" t="s">
         <v>109</v>
       </c>
@@ -2437,7 +2511,7 @@
         <v>102</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>119</v>
@@ -2451,10 +2525,10 @@
       <c r="H15" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J15" s="35">
+      <c r="J15" s="60">
         <v>0.95</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2483,10 +2557,10 @@
       <c r="H16" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="13">
         <v>0.9</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2515,10 +2589,10 @@
       <c r="H17" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="13">
         <v>0.95</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2547,10 +2621,10 @@
       <c r="H18" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="13">
         <v>0.95</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2565,7 +2639,7 @@
         <v>102</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>119</v>
@@ -2579,14 +2653,14 @@
       <c r="H19" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="13">
         <v>0.91</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="16">
+      <c r="K19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="14" t="s">
         <v>112</v>
       </c>
@@ -2597,7 +2671,7 @@
         <v>102</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>119</v>
@@ -2611,14 +2685,14 @@
       <c r="H20" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="13">
         <v>0.23</v>
       </c>
-      <c r="K20" s="35">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="16">
+      <c r="K20" s="61">
+        <v>-2.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="14" t="s">
         <v>113</v>
       </c>
@@ -2629,7 +2703,7 @@
         <v>240</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>119</v>
@@ -2643,10 +2717,10 @@
       <c r="H21" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J21" s="35">
-        <v>0.36</v>
-      </c>
-      <c r="K21" s="35">
+      <c r="J21" s="61">
+        <v>0.33</v>
+      </c>
+      <c r="K21" s="60">
         <v>-2</v>
       </c>
     </row>
@@ -2664,7 +2738,7 @@
         <v>119</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>119</v>
@@ -2678,14 +2752,14 @@
       <c r="I22">
         <v>4</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="13">
         <v>0.75</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="16">
+      <c r="K22" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="5" t="s">
         <v>121</v>
       </c>
@@ -2696,7 +2770,7 @@
         <v>99</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>119</v>
@@ -2710,14 +2784,14 @@
       <c r="H23" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="13">
         <v>0.23</v>
       </c>
-      <c r="K23" s="35">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="16">
+      <c r="K23" s="61">
+        <v>-2.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
         <v>231</v>
       </c>
@@ -2728,7 +2802,7 @@
         <v>240</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>119</v>
@@ -2742,10 +2816,10 @@
       <c r="H24" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J24" s="35">
-        <v>0.36</v>
-      </c>
-      <c r="K24" s="35">
+      <c r="J24" s="61">
+        <v>0.33</v>
+      </c>
+      <c r="K24" s="60">
         <v>-2</v>
       </c>
     </row>
@@ -2775,7 +2849,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2783,7 +2857,7 @@
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
@@ -2848,10 +2922,10 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="18">
         <v>29.1</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2876,7 +2950,7 @@
       <c r="A4" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="18">
         <v>85</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -2898,10 +2972,10 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="18">
         <v>23.3</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -2923,460 +2997,460 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="33">
         <v>87</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="34">
         <v>54.1</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="5">
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35">
         <v>35</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="35" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="36">
         <v>30</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="35">
         <v>54.1</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5">
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35">
         <v>35</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="35" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="36">
         <v>23.2</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="35">
         <v>20</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5">
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35">
         <v>30</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="35" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="36">
         <v>93.6</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="35">
         <v>32.6</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="5">
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35">
         <v>100</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="35" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="36">
         <v>61.9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="35">
         <v>35.299999999999997</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8">
+      <c r="F10" s="35"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34">
         <v>45</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="35" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="36">
         <v>50</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="35">
         <v>80</v>
       </c>
-      <c r="E11" s="34" t="s">
-        <v>256</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="5">
+      <c r="E11" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="F11" s="35"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35">
         <v>100</v>
       </c>
-      <c r="I11" s="34" t="s">
-        <v>254</v>
+      <c r="I11" s="56" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="36">
         <v>48.5</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="35">
         <v>50</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="5">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35">
         <v>30</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="35" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="38">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="40">
         <v>85</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14">
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40">
         <v>15</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="40" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="38">
         <v>50</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="40">
         <v>80</v>
       </c>
-      <c r="E14" s="34" t="s">
-        <v>256</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14">
+      <c r="E14" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40">
         <v>100</v>
       </c>
-      <c r="I14" s="34" t="s">
-        <v>254</v>
+      <c r="I14" s="57" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="38">
         <v>61.9</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="40">
         <v>35.299999999999997</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15">
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="32">
         <v>45</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="38">
         <v>30</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="39">
         <v>39.4</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14">
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40">
         <v>40</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="38">
         <v>87</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="39">
         <v>51.7</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14">
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40">
         <v>45</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="38">
         <v>87</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="40">
         <v>54.1</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14">
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40">
         <v>30</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="38">
         <v>30</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="40">
         <v>42.47</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="15">
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="32">
         <v>55</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="40" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:9">
+      <c r="A20" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="38">
         <v>23.2</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="40">
         <v>20</v>
       </c>
-      <c r="E20" s="35" t="s">
-        <v>255</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14">
+      <c r="E20" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40">
         <v>30</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="38">
         <v>48.5</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="40">
         <v>50</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14">
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40">
         <v>30</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B22" s="36">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="34">
         <v>85</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8">
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34">
         <v>15</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="35" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="16">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:9">
+      <c r="A23" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="36">
         <v>23.2</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="35">
         <v>20</v>
       </c>
-      <c r="E23" s="35" t="s">
-        <v>255</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8">
+      <c r="E23" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="F23" s="35"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34">
         <v>30</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="35" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="19">
         <v>46</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -3398,8 +3472,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E20" r:id="rId1" xr:uid="{3CEF7FAA-4504-5F4D-958D-96854D43F066}"/>
+    <hyperlink ref="E23" r:id="rId2" xr:uid="{D13488A1-ADCB-664A-92F0-99D61413F0F6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3408,7 +3486,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3417,11 +3495,12 @@
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.1640625" customWidth="1"/>
@@ -3503,8 +3582,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" s="41" t="s">
         <v>103</v>
       </c>
       <c r="B3" s="5"/>
@@ -3529,21 +3608,22 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="16">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="41" t="s">
         <v>237</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="E4" s="32">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="27">
+        <v>12.9</v>
+      </c>
+      <c r="F4" s="24">
+        <v>0</v>
+      </c>
+      <c r="G4" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="29">
         <v>0.6</v>
       </c>
       <c r="I4">
@@ -3554,32 +3634,32 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="16">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="41" t="s">
         <v>104</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="E5" s="32">
-        <v>42</v>
+      <c r="E5" s="48">
+        <v>43.6</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="H5" s="35">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16">
-      <c r="A6" s="36" t="s">
+      <c r="G5" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" s="46">
+        <v>0</v>
+      </c>
+      <c r="I5" s="47">
+        <v>0</v>
+      </c>
+      <c r="J5" s="45" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="41" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="5"/>
@@ -3603,8 +3683,8 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:12">
+      <c r="A7" s="41" t="s">
         <v>238</v>
       </c>
       <c r="B7" s="5"/>
@@ -3628,8 +3708,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16">
-      <c r="A8" s="36" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" s="41" t="s">
         <v>106</v>
       </c>
       <c r="B8" s="5"/>
@@ -3653,13 +3733,13 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16">
-      <c r="A9" s="36" t="s">
+    <row r="9" spans="1:12">
+      <c r="A9" s="41" t="s">
         <v>186</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="E9" s="26">
+      <c r="E9" s="19">
         <v>119</v>
       </c>
       <c r="F9">
@@ -3678,13 +3758,13 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:12">
+      <c r="A10" s="41" t="s">
         <v>193</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="E10" s="28">
+      <c r="E10" s="20">
         <v>123</v>
       </c>
       <c r="F10">
@@ -3704,12 +3784,12 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="16">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="41" t="s">
         <v>202</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="E11" s="32">
+      <c r="E11" s="52">
         <v>3</v>
       </c>
       <c r="F11">
@@ -3718,18 +3798,18 @@
       <c r="G11" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="H11" s="34">
-        <v>13.9</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="16">
-      <c r="A12" s="36" t="s">
+      <c r="H11" s="53">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="I11" s="43">
+        <v>0</v>
+      </c>
+      <c r="J11" s="54" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="41" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="5"/>
@@ -3743,312 +3823,332 @@
       <c r="G12" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H12" s="17">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17">
+      <c r="H12" s="15">
+        <v>0</v>
+      </c>
+      <c r="I12" s="15">
         <v>0</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16">
-      <c r="A13" s="36" t="s">
+    <row r="13" spans="1:12">
+      <c r="A13" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="31">
         <v>1004</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="31">
         <v>-1.97</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="31">
         <v>25.1</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="31">
         <v>-1.97</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H13" s="31">
+        <v>0</v>
+      </c>
+      <c r="I13" s="31">
+        <v>0</v>
+      </c>
+      <c r="J13" s="31" t="s">
         <v>244</v>
       </c>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
     </row>
     <row r="14" spans="1:12" ht="16">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="32">
-        <v>1179</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E14" s="32">
+      <c r="B14" s="55">
+        <v>1439</v>
+      </c>
+      <c r="C14" s="43">
+        <v>0</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14" s="51">
         <v>3</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="43">
+        <v>0</v>
+      </c>
+      <c r="G14" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="H14" s="34">
-        <v>13.9</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="16">
-      <c r="A15" s="36" t="s">
+      <c r="H14" s="53">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="I14" s="43">
+        <v>0</v>
+      </c>
+      <c r="J14" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="31">
         <v>4247</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="31">
         <v>-0.53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="31">
         <v>123</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F15" s="31">
+        <v>0</v>
+      </c>
+      <c r="G15" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="31">
         <v>1.31</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="I15" s="31">
+        <v>0</v>
+      </c>
+      <c r="J15" s="31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="16">
-      <c r="A16" s="36" t="s">
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="42" t="s">
         <v>176</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="31">
         <v>4099</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="31">
         <v>-0.35</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="31">
         <v>39.700000000000003</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F16" s="31">
+        <v>0</v>
+      </c>
+      <c r="G16" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="31">
         <v>1.22</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="I16" s="31">
+        <v>0</v>
+      </c>
+      <c r="J16" s="31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="16">
-      <c r="A17" s="36" t="s">
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="31">
         <v>1008</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="31">
         <v>-0.4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E17">
-        <v>13</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="E17" s="31">
+        <v>12.9</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0</v>
+      </c>
+      <c r="G17" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="31">
         <v>0.6</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="I17" s="31">
+        <v>0</v>
+      </c>
+      <c r="J17" s="31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="16">
-      <c r="A18" s="36" t="s">
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="31">
         <v>1008</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="31">
         <v>-0.4</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="31">
         <v>12.9</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F18" s="31">
+        <v>0</v>
+      </c>
+      <c r="G18" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="31">
         <v>0.6</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="I18" s="31">
+        <v>0</v>
+      </c>
+      <c r="J18" s="31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="16">
-      <c r="A19" s="36" t="s">
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="31">
         <v>925</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="31">
         <v>-0.41</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="31">
         <v>11.4</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="F19" s="31">
+        <v>0</v>
+      </c>
+      <c r="G19" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="31">
         <v>1.25</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="I19" s="31">
+        <v>0</v>
+      </c>
+      <c r="J19" s="31" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="16">
-      <c r="A20" s="36" t="s">
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="31">
         <v>1095</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="31">
         <v>-1.86</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="31">
         <v>12.8</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="31">
         <v>-1.86</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="H20" s="31">
+        <v>0</v>
+      </c>
+      <c r="I20" s="31">
+        <v>0</v>
+      </c>
+      <c r="J20" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="31">
         <v>0.08</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="31" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="16">
-      <c r="A21" s="36" t="s">
+    <row r="21" spans="1:12">
+      <c r="A21" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="31">
         <v>3245</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="31">
         <v>-1.7</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="31">
         <v>88.6</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="31">
         <v>-1.88</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="H21" s="31">
+        <v>0</v>
+      </c>
+      <c r="I21" s="31">
+        <v>0</v>
+      </c>
+      <c r="J21" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="31">
         <v>0.08</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="31" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="16">
-      <c r="A22" s="36" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="41" t="s">
         <v>120</v>
       </c>
       <c r="B22">
@@ -4079,8 +4179,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16">
-      <c r="A23" s="36" t="s">
+    <row r="23" spans="1:12">
+      <c r="A23" s="41" t="s">
         <v>121</v>
       </c>
       <c r="B23">
@@ -4117,8 +4217,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="16">
-      <c r="A24" s="36" t="s">
+    <row r="24" spans="1:12">
+      <c r="A24" s="41" t="s">
         <v>231</v>
       </c>
       <c r="B24">
@@ -4163,7 +4263,7 @@
       <c r="L25" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4174,12 +4274,12 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
@@ -4335,128 +4435,176 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="H12">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="H12" s="49"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31">
         <v>2025</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="H13">
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31">
+        <v>300</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31">
         <v>2025</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14">
-        <v>300</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31">
+        <v>2025</v>
+      </c>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31">
+        <v>2025</v>
+      </c>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="30">
+        <v>0.67</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31">
+        <v>2025</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31">
+        <v>2025</v>
+      </c>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31">
+        <v>2025</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31">
+        <v>40000</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31">
+        <v>2025</v>
+      </c>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31">
+        <v>5200</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="H14">
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31">
         <v>2025</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="H15">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B16" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="H16">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B17" s="14">
-        <v>0.67</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="H17">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="H18">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="H19">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20">
-        <v>40000</v>
-      </c>
-      <c r="E20" t="s">
-        <v>245</v>
-      </c>
-      <c r="H20">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21">
-        <v>5200</v>
-      </c>
-      <c r="E21" t="s">
-        <v>234</v>
-      </c>
-      <c r="H21">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="5" t="s">
         <v>120</v>
       </c>
@@ -4464,7 +4612,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10">
       <c r="A23" s="5" t="s">
         <v>121</v>
       </c>
@@ -4478,7 +4626,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:10">
       <c r="A24" s="5" t="s">
         <v>231</v>
       </c>
@@ -4496,8 +4644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4700,7 +4848,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4823,58 +4971,58 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="22">
+      <c r="A9" s="39">
         <v>2035</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="39">
         <v>16100</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="39" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="22">
+      <c r="A10" s="39">
         <v>2040</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="39">
         <v>16100</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="39" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="22">
+      <c r="A11" s="39">
         <v>2045</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="39">
         <v>16100</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="39" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="22">
+      <c r="A12" s="39">
         <v>2050</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="39">
         <v>16100</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="39" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4944,7 +5092,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4970,9 +5118,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>0.36399999999999999</v>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="23">
+        <v>0.41860000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -4984,8 +5132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="I232" sqref="I232"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9950,7 +10098,7 @@
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="17" t="s">
         <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -10270,8 +10418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:Q16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10413,16 +10561,16 @@
       <c r="C3" t="s">
         <v>166</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="13">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="62">
+        <v>0</v>
+      </c>
+      <c r="G3" s="62">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -10460,16 +10608,16 @@
       <c r="C4" t="s">
         <v>99</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="13">
         <v>0.4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="F4" s="62">
+        <v>0</v>
+      </c>
+      <c r="G4" s="62">
         <v>0</v>
       </c>
       <c r="H4" s="2"/>
@@ -10505,16 +10653,16 @@
       <c r="C5" t="s">
         <v>172</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="13">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="62">
+        <v>0</v>
+      </c>
+      <c r="G5" s="62">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -10546,22 +10694,22 @@
       <c r="A6" t="s">
         <v>171</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="62">
+        <v>0</v>
+      </c>
+      <c r="G6" s="62">
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -10593,19 +10741,20 @@
       <c r="A7" t="s">
         <v>100</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="62">
+        <v>0</v>
+      </c>
+      <c r="G7" s="62">
         <v>0</v>
       </c>
       <c r="H7" s="2"/>
@@ -10633,22 +10782,22 @@
       <c r="A8" t="s">
         <v>169</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="62">
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -10680,22 +10829,22 @@
       <c r="A9" t="s">
         <v>168</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="62">
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -10727,19 +10876,20 @@
       <c r="A10" t="s">
         <v>225</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="20">
+      <c r="D10" s="13">
+        <v>0</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13">
         <v>0.50697570000000003</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="62">
         <v>20</v>
       </c>
       <c r="H10" s="2"/>
@@ -10768,19 +10918,20 @@
       <c r="A11" t="s">
         <v>227</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="20">
+      <c r="D11" s="13">
+        <v>0</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13">
         <v>0.37906770000000001</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="62">
         <v>20</v>
       </c>
       <c r="H11" s="2"/>
@@ -10808,19 +10959,20 @@
       <c r="A12" t="s">
         <v>226</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="20">
+      <c r="D12" s="13">
+        <v>0</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13">
         <v>0.28218300000000002</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="62">
         <v>20</v>
       </c>
       <c r="H12" s="2"/>
@@ -10848,19 +11000,20 @@
       <c r="A13" t="s">
         <v>228</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="20">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="D13" s="13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="62">
         <v>0</v>
       </c>
       <c r="H13" s="2"/>
@@ -10895,13 +11048,14 @@
       <c r="C14" t="s">
         <v>174</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="20">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="62">
         <v>0</v>
       </c>
       <c r="H14" s="2"/>
@@ -10935,13 +11089,14 @@
       <c r="C15" t="s">
         <v>175</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="20">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="62">
         <v>0</v>
       </c>
       <c r="H15" s="2"/>
@@ -10975,13 +11130,14 @@
       <c r="C16" t="s">
         <v>102</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
+      <c r="D16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13">
+        <v>0</v>
+      </c>
+      <c r="G16" s="13">
         <v>0</v>
       </c>
       <c r="I16">
@@ -11013,8 +11169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11277,15 +11433,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28912B5-8590-412C-8145-960D60FAEF13}">
   <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12895,10 +13051,10 @@
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="C149" s="21"/>
+      <c r="C149" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12907,9 +13063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -12951,7 +13105,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D9"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -12974,16 +13128,16 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="13" t="s">
         <v>212</v>
       </c>
       <c r="E2" t="s">
@@ -12991,100 +13145,100 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="19">
+      <c r="A3" s="13">
         <v>2018</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="64">
         <v>1000000</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="19">
+      <c r="A4" s="13">
         <v>2025</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="65">
         <v>23800</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="19">
+      <c r="A5" s="13">
         <v>2030</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C5" s="19">
-        <v>19600</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="65">
+        <v>11900</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="19">
+      <c r="A6" s="13">
         <v>2035</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C6" s="19">
-        <v>14700</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="65">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="19">
+      <c r="A7" s="13">
         <v>2040</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="19">
-        <v>9800</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="65">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="19">
+      <c r="A8" s="13">
         <v>2045</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C8" s="19">
-        <v>4900</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="65">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="19">
+      <c r="A9" s="13">
         <v>2050</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="19">
-        <v>0</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="65">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>223</v>
       </c>
     </row>

</xml_diff>